<commit_message>
gw: lf tas1 update forms
</commit_message>
<xml_diff>
--- a/LF/TAS/Guinee Bissau/2023/gw_lf_tas1_202310_1_sites.xlsx
+++ b/LF/TAS/Guinee Bissau/2023/gw_lf_tas1_202310_1_sites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\LF\TAS\Guinee Bissau\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{528E11F0-7B98-462D-9E17-B7D9BFBE7083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C28773-D148-4F55-AC60-097E4F164523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -609,10 +609,10 @@
     <t>select_one eu</t>
   </si>
   <si>
-    <t>(Fev 2024) 1. TAS1 FL - Formulário do site</t>
-  </si>
-  <si>
-    <t>gw_lf_tas1_202402_1_sites</t>
+    <t>(Fev 2024) 1. TAS1 FL - Formulário do site V2</t>
+  </si>
+  <si>
+    <t>gw_lf_tas1_202402_1_sites_v2</t>
   </si>
 </sst>
 </file>
@@ -4565,7 +4565,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>

</xml_diff>